<commit_message>
facts: rename excel sheet "movies" to "movie"
</commit_message>
<xml_diff>
--- a/facts/step4/all-titles.xlsx
+++ b/facts/step4/all-titles.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Dropbox\Coding\marvelsnap-in-movies\facts\step3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Dropbox\Coding\marvelsnap-in-movies\facts\step4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F657AC93-64EE-4AB4-A265-433BF891EC86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA71F8F-8BBE-45B0-9010-D8454E9763C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
   </bookViews>
   <sheets>
-    <sheet name="movies" sheetId="1" r:id="rId1"/>
+    <sheet name="movie" sheetId="1" r:id="rId1"/>
     <sheet name="live-action-tv-series" sheetId="2" r:id="rId2"/>
     <sheet name="animated-tv-series" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -1262,7 +1262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF7CD8B-2C72-4367-8653-A42EAAA710BE}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
@@ -2829,8 +2829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3300BA2F-EA0D-4163-B184-5C04F63CD480}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
facts: restructure: use "label" instead of "continuity"
</commit_message>
<xml_diff>
--- a/facts/step4/all-titles.xlsx
+++ b/facts/step4/all-titles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Dropbox\Coding\marvelsnap-in-movies\facts\step4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA71F8F-8BBE-45B0-9010-D8454E9763C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E7DDD2-E3B7-43B9-8F77-49391857DA30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
   </bookViews>
   <sheets>
     <sheet name="movie" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="291">
   <si>
     <t>Blade</t>
   </si>
@@ -568,9 +568,6 @@
     <t>tobey-spiderman</t>
   </si>
   <si>
-    <t>continuity</t>
-  </si>
-  <si>
     <t>fox-fantastic-four</t>
   </si>
   <si>
@@ -793,12 +790,6 @@
     <t>2023</t>
   </si>
   <si>
-    <t>isAnime</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>2021</t>
   </si>
   <si>
@@ -823,9 +814,6 @@
     <t>https://en.wikipedia.org/wiki/Spider-Man:_Across_the_Spider-Verse</t>
   </si>
   <si>
-    <t>mcu-netflix</t>
-  </si>
-  <si>
     <t>Spider-Man: The Animated Series</t>
   </si>
   <si>
@@ -908,6 +896,21 @@
   </si>
   <si>
     <t>1996–1997</t>
+  </si>
+  <si>
+    <t>fox-x-men,deadpool</t>
+  </si>
+  <si>
+    <t>ssu,venom</t>
+  </si>
+  <si>
+    <t>mcu,netflix</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>anime</t>
   </si>
 </sst>
 </file>
@@ -1262,8 +1265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF7CD8B-2C72-4367-8653-A42EAAA710BE}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1282,10 +1285,10 @@
         <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D1" t="s">
-        <v>176</v>
+        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1296,7 +1299,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D2" t="s">
         <v>174</v>
@@ -1310,10 +1313,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1324,7 +1327,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D4" t="s">
         <v>174</v>
@@ -1338,7 +1341,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D5" t="s">
         <v>175</v>
@@ -1352,10 +1355,10 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1366,10 +1369,10 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1380,7 +1383,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1391,7 +1394,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1402,7 +1405,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D10" t="s">
         <v>175</v>
@@ -1416,7 +1419,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D11" t="s">
         <v>174</v>
@@ -1430,10 +1433,10 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1444,10 +1447,10 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1458,10 +1461,10 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1472,10 +1475,10 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1486,7 +1489,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D16" t="s">
         <v>175</v>
@@ -1500,10 +1503,10 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1514,7 +1517,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D18" t="s">
         <v>114</v>
@@ -1528,7 +1531,7 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D19" t="s">
         <v>114</v>
@@ -1542,7 +1545,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1553,10 +1556,10 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1567,7 +1570,7 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D22" t="s">
         <v>114</v>
@@ -1581,7 +1584,7 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D23" t="s">
         <v>114</v>
@@ -1595,10 +1598,10 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1609,7 +1612,7 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D25" t="s">
         <v>114</v>
@@ -1623,10 +1626,10 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1637,7 +1640,7 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D27" t="s">
         <v>114</v>
@@ -1651,10 +1654,10 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D28" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1665,7 +1668,7 @@
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D29" t="s">
         <v>114</v>
@@ -1679,10 +1682,10 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D30" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1693,7 +1696,7 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D31" t="s">
         <v>114</v>
@@ -1707,7 +1710,7 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D32" t="s">
         <v>114</v>
@@ -1721,10 +1724,10 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1735,10 +1738,10 @@
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D34" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1749,7 +1752,7 @@
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D35" t="s">
         <v>114</v>
@@ -1763,7 +1766,7 @@
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D36" t="s">
         <v>114</v>
@@ -1777,7 +1780,7 @@
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D37" t="s">
         <v>114</v>
@@ -1791,7 +1794,7 @@
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1802,10 +1805,10 @@
         <v>36</v>
       </c>
       <c r="C39" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D39" t="s">
-        <v>179</v>
+        <v>286</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1816,7 +1819,7 @@
         <v>37</v>
       </c>
       <c r="C40" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D40" t="s">
         <v>114</v>
@@ -1830,10 +1833,10 @@
         <v>38</v>
       </c>
       <c r="C41" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D41" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1844,7 +1847,7 @@
         <v>39</v>
       </c>
       <c r="C42" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D42" t="s">
         <v>114</v>
@@ -1858,10 +1861,10 @@
         <v>40</v>
       </c>
       <c r="C43" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D43" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1872,7 +1875,7 @@
         <v>41</v>
       </c>
       <c r="C44" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D44" t="s">
         <v>114</v>
@@ -1886,7 +1889,7 @@
         <v>42</v>
       </c>
       <c r="C45" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D45" t="s">
         <v>114</v>
@@ -1900,7 +1903,7 @@
         <v>43</v>
       </c>
       <c r="C46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D46" t="s">
         <v>114</v>
@@ -1914,7 +1917,7 @@
         <v>44</v>
       </c>
       <c r="C47" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D47" t="s">
         <v>114</v>
@@ -1928,7 +1931,7 @@
         <v>45</v>
       </c>
       <c r="C48" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D48" t="s">
         <v>114</v>
@@ -1942,10 +1945,10 @@
         <v>46</v>
       </c>
       <c r="C49" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D49" t="s">
-        <v>179</v>
+        <v>286</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1956,7 +1959,7 @@
         <v>47</v>
       </c>
       <c r="C50" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D50" t="s">
         <v>114</v>
@@ -1970,24 +1973,24 @@
         <v>48</v>
       </c>
       <c r="C51" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D51" t="s">
-        <v>182</v>
+        <v>287</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B52" t="s">
+        <v>253</v>
+      </c>
+      <c r="C52" t="s">
+        <v>254</v>
+      </c>
+      <c r="D52" t="s">
         <v>255</v>
-      </c>
-      <c r="B52" t="s">
-        <v>256</v>
-      </c>
-      <c r="C52" t="s">
-        <v>257</v>
-      </c>
-      <c r="D52" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1998,7 +2001,7 @@
         <v>49</v>
       </c>
       <c r="C53" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D53" t="s">
         <v>114</v>
@@ -2012,7 +2015,7 @@
         <v>50</v>
       </c>
       <c r="C54" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D54" t="s">
         <v>114</v>
@@ -2026,10 +2029,10 @@
         <v>51</v>
       </c>
       <c r="C55" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D55" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -2040,7 +2043,7 @@
         <v>52</v>
       </c>
       <c r="C56" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D56" t="s">
         <v>114</v>
@@ -2054,10 +2057,10 @@
         <v>53</v>
       </c>
       <c r="C57" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D57" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -2068,7 +2071,7 @@
         <v>54</v>
       </c>
       <c r="C58" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D58" t="s">
         <v>114</v>
@@ -2082,7 +2085,7 @@
         <v>55</v>
       </c>
       <c r="C59" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D59" t="s">
         <v>114</v>
@@ -2096,10 +2099,10 @@
         <v>56</v>
       </c>
       <c r="C60" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D60" t="s">
-        <v>182</v>
+        <v>287</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -2110,7 +2113,7 @@
         <v>57</v>
       </c>
       <c r="C61" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D61" t="s">
         <v>114</v>
@@ -2124,7 +2127,7 @@
         <v>58</v>
       </c>
       <c r="C62" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D62" t="s">
         <v>114</v>
@@ -2138,10 +2141,10 @@
         <v>59</v>
       </c>
       <c r="C63" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D63" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -2152,7 +2155,7 @@
         <v>60</v>
       </c>
       <c r="C64" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D64" t="s">
         <v>114</v>
@@ -2166,7 +2169,7 @@
         <v>61</v>
       </c>
       <c r="C65" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D65" t="s">
         <v>114</v>
@@ -2180,7 +2183,7 @@
         <v>62</v>
       </c>
       <c r="C66" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D66" t="s">
         <v>114</v>
@@ -2194,7 +2197,7 @@
         <v>63</v>
       </c>
       <c r="C67" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D67" t="s">
         <v>114</v>
@@ -2208,7 +2211,7 @@
         <v>64</v>
       </c>
       <c r="C68" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D68" t="s">
         <v>114</v>
@@ -2216,16 +2219,16 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B69" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C69" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D69" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -2307,7 +2310,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2328,7 +2331,7 @@
         <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D1" t="s">
         <v>112</v>
@@ -2337,7 +2340,7 @@
         <v>113</v>
       </c>
       <c r="F1" t="s">
-        <v>176</v>
+        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2362,7 +2365,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B3" t="s">
         <v>68</v>
@@ -2382,7 +2385,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B4" t="s">
         <v>69</v>
@@ -2397,12 +2400,12 @@
         <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>261</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -2417,12 +2420,12 @@
         <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>261</v>
+        <v>288</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B6" t="s">
         <v>70</v>
@@ -2437,12 +2440,12 @@
         <v>39</v>
       </c>
       <c r="F6" t="s">
-        <v>261</v>
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B7" t="s">
         <v>71</v>
@@ -2457,12 +2460,12 @@
         <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>261</v>
+        <v>288</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B8" t="s">
         <v>72</v>
@@ -2479,7 +2482,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B9" t="s">
         <v>73</v>
@@ -2494,7 +2497,7 @@
         <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>261</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -2514,7 +2517,7 @@
         <v>8</v>
       </c>
       <c r="F10" t="s">
-        <v>261</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2539,7 +2542,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B12" t="s">
         <v>76</v>
@@ -2556,7 +2559,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -2571,12 +2574,12 @@
         <v>26</v>
       </c>
       <c r="F13" t="s">
-        <v>261</v>
+        <v>288</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B14" t="s">
         <v>77</v>
@@ -2596,7 +2599,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B15" t="s">
         <v>78</v>
@@ -2693,7 +2696,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B20" t="s">
         <v>86</v>
@@ -2773,7 +2776,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B24" t="s">
         <v>87</v>
@@ -2829,8 +2832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3300BA2F-EA0D-4163-B184-5C04F63CD480}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2860,15 +2863,15 @@
         <v>113</v>
       </c>
       <c r="F1" t="s">
-        <v>251</v>
+        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C2" t="s">
         <v>142</v>
@@ -2882,10 +2885,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B3" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C3" t="s">
         <v>143</v>
@@ -2899,7 +2902,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -2916,10 +2919,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B5" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C5" t="s">
         <v>145</v>
@@ -2933,7 +2936,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
@@ -3001,7 +3004,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B10" t="s">
         <v>120</v>
@@ -3035,7 +3038,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B12" t="s">
         <v>122</v>
@@ -3052,7 +3055,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B13" t="s">
         <v>123</v>
@@ -3086,7 +3089,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B15" t="s">
         <v>125</v>
@@ -3103,7 +3106,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B16" t="s">
         <v>126</v>
@@ -3120,7 +3123,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B17" t="s">
         <v>127</v>
@@ -3137,7 +3140,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B18" t="s">
         <v>128</v>
@@ -3152,12 +3155,12 @@
         <v>12</v>
       </c>
       <c r="F18" t="s">
-        <v>252</v>
+        <v>290</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B19" t="s">
         <v>129</v>
@@ -3172,12 +3175,12 @@
         <v>12</v>
       </c>
       <c r="F19" t="s">
-        <v>252</v>
+        <v>290</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B20" t="s">
         <v>130</v>
@@ -3192,12 +3195,12 @@
         <v>12</v>
       </c>
       <c r="F20" t="s">
-        <v>252</v>
+        <v>290</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B21" t="s">
         <v>131</v>
@@ -3212,12 +3215,12 @@
         <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>252</v>
+        <v>290</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B22" t="s">
         <v>132</v>
@@ -3234,7 +3237,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B23" t="s">
         <v>133</v>
@@ -3251,7 +3254,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B24" t="s">
         <v>134</v>
@@ -3268,7 +3271,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B25" t="s">
         <v>135</v>
@@ -3283,12 +3286,12 @@
         <v>51</v>
       </c>
       <c r="F25" t="s">
-        <v>252</v>
+        <v>290</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B26" t="s">
         <v>33</v>
@@ -3305,7 +3308,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B27" t="s">
         <v>136</v>
@@ -3320,12 +3323,12 @@
         <v>39</v>
       </c>
       <c r="F27" t="s">
-        <v>252</v>
+        <v>290</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B28" t="s">
         <v>137</v>
@@ -3359,7 +3362,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B30" t="s">
         <v>139</v>
@@ -3376,7 +3379,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B31" t="s">
         <v>140</v>
@@ -3393,7 +3396,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B32" t="s">
         <v>141</v>

</xml_diff>

<commit_message>
facts: add tv specials
</commit_message>
<xml_diff>
--- a/facts/step4/all-titles.xlsx
+++ b/facts/step4/all-titles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Dropbox\Coding\marvelsnap-on-screen\facts\step4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7464A004-CF80-4B5C-9D96-005F6D0E035B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31C2363-8278-4926-B16B-D2024AFC0EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
   </bookViews>
   <sheets>
     <sheet name="movie" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="302">
   <si>
     <t>Blade</t>
   </si>
@@ -932,6 +932,18 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/Echo_(miniseries)</t>
+  </si>
+  <si>
+    <t>Werewolf by Night</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Werewolf_by_Night_(TV_special)</t>
+  </si>
+  <si>
+    <t>The Guardians of the Galaxy Holiday Special</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/The_Guardians_of_the_Galaxy_Holiday_Special</t>
   </si>
 </sst>
 </file>
@@ -1290,10 +1302,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF7CD8B-2C72-4367-8653-A42EAAA710BE}">
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2817,13 +2829,13 @@
         <v>290</v>
       </c>
       <c r="B67" s="1">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C67" t="s">
-        <v>63</v>
+        <v>298</v>
       </c>
       <c r="D67" t="s">
-        <v>246</v>
+        <v>299</v>
       </c>
       <c r="E67" t="s">
         <v>113</v>
@@ -2840,13 +2852,13 @@
         <v>290</v>
       </c>
       <c r="B68" s="1">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C68" t="s">
-        <v>64</v>
+        <v>300</v>
       </c>
       <c r="D68" t="s">
-        <v>247</v>
+        <v>301</v>
       </c>
       <c r="E68" t="s">
         <v>113</v>
@@ -2862,17 +2874,17 @@
       <c r="A69" t="s">
         <v>290</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>248</v>
+      <c r="B69" s="1">
+        <v>2023</v>
       </c>
       <c r="C69" t="s">
-        <v>254</v>
+        <v>63</v>
       </c>
       <c r="D69" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="E69" t="s">
-        <v>293</v>
+        <v>113</v>
       </c>
       <c r="F69">
         <v>0</v>
@@ -2885,22 +2897,68 @@
       <c r="A70" t="s">
         <v>290</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="1">
+        <v>2023</v>
+      </c>
+      <c r="C70" t="s">
+        <v>64</v>
+      </c>
+      <c r="D70" t="s">
+        <v>247</v>
+      </c>
+      <c r="E70" t="s">
+        <v>113</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>290</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C71" t="s">
+        <v>254</v>
+      </c>
+      <c r="D71" t="s">
+        <v>255</v>
+      </c>
+      <c r="E71" t="s">
+        <v>293</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>290</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C72" t="s">
         <v>294</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D72" t="s">
         <v>295</v>
       </c>
-      <c r="E70" t="s">
-        <v>113</v>
-      </c>
-      <c r="F70">
-        <v>0</v>
-      </c>
-      <c r="G70">
+      <c r="E72" t="s">
+        <v>113</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
         <v>1</v>
       </c>
     </row>
@@ -2970,8 +3028,8 @@
     <hyperlink ref="C64" r:id="rId62" tooltip="Doctor Strange in the Multiverse of Madness" display="https://en.wikipedia.org/wiki/Doctor_Strange_in_the_Multiverse_of_Madness" xr:uid="{CDBEA5E1-B291-47EA-A287-6F70E8CAB7B1}"/>
     <hyperlink ref="C65" r:id="rId63" tooltip="Thor: Love and Thunder" display="https://en.wikipedia.org/wiki/Thor:_Love_and_Thunder" xr:uid="{3AB74F2C-F69C-4D2D-BDED-4A813BF8BFEE}"/>
     <hyperlink ref="C66" r:id="rId64" tooltip="Black Panther: Wakanda Forever" display="https://en.wikipedia.org/wiki/Black_Panther:_Wakanda_Forever" xr:uid="{ADC5FD84-B490-48F8-9C96-439E4409564C}"/>
-    <hyperlink ref="C67" r:id="rId65" tooltip="Ant-Man and the Wasp: Quantumania" display="https://en.wikipedia.org/wiki/Ant-Man_and_the_Wasp:_Quantumania" xr:uid="{B07888B3-15E9-4AFF-902A-DBEAA382600F}"/>
-    <hyperlink ref="C68" r:id="rId66" tooltip="Guardians of the Galaxy Vol. 3" display="https://en.wikipedia.org/wiki/Guardians_of_the_Galaxy_Vol._3" xr:uid="{950701D0-7631-4DC3-B474-8A55F81C297D}"/>
+    <hyperlink ref="C69" r:id="rId65" tooltip="Ant-Man and the Wasp: Quantumania" display="https://en.wikipedia.org/wiki/Ant-Man_and_the_Wasp:_Quantumania" xr:uid="{B07888B3-15E9-4AFF-902A-DBEAA382600F}"/>
+    <hyperlink ref="C70" r:id="rId66" tooltip="Guardians of the Galaxy Vol. 3" display="https://en.wikipedia.org/wiki/Guardians_of_the_Galaxy_Vol._3" xr:uid="{950701D0-7631-4DC3-B474-8A55F81C297D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId67"/>
@@ -2982,7 +3040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A614F1-7948-4686-8AED-21AFC5640E8C}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add "I am Groot"
</commit_message>
<xml_diff>
--- a/facts/step4/all-titles.xlsx
+++ b/facts/step4/all-titles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Dropbox\Coding\marvelsnap-on-screen\facts\step4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31C2363-8278-4926-B16B-D2024AFC0EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DF7A9F-D214-4CB8-8C40-7DA7A9E51B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
   </bookViews>
   <sheets>
     <sheet name="movie" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="305">
   <si>
     <t>Blade</t>
   </si>
@@ -944,6 +944,15 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/The_Guardians_of_the_Galaxy_Holiday_Special</t>
+  </si>
+  <si>
+    <t>2022-2023</t>
+  </si>
+  <si>
+    <t>I am Groot</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/I_Am_Groot</t>
   </si>
 </sst>
 </file>
@@ -1304,7 +1313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF7CD8B-2C72-4367-8653-A42EAAA710BE}">
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+    <sheetView topLeftCell="A48" workbookViewId="0">
       <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
@@ -3041,7 +3050,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3658,10 +3667,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3300BA2F-EA0D-4163-B184-5C04F63CD480}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4320,19 +4329,39 @@
       <c r="A32" t="s">
         <v>291</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
+        <v>302</v>
+      </c>
+      <c r="C32" t="s">
+        <v>303</v>
+      </c>
+      <c r="D32" t="s">
+        <v>304</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>291</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>140</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>171</v>
       </c>
-      <c r="F32">
-        <v>1</v>
-      </c>
-      <c r="G32">
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
         <v>17</v>
       </c>
     </row>
@@ -4369,7 +4398,7 @@
     <hyperlink ref="C29" r:id="rId29" tooltip="M.O.D.O.K. (TV series)" display="https://en.wikipedia.org/wiki/M.O.D.O.K._(TV_series)" xr:uid="{2534FEF3-0AF4-4829-A137-17AD8F95F95C}"/>
     <hyperlink ref="C30" r:id="rId30" tooltip="Spidey and His Amazing Friends (2021 TV series)" display="https://en.wikipedia.org/wiki/Spidey_and_His_Amazing_Friends_(2021_TV_series)" xr:uid="{4806F038-3D39-42C6-B9FC-4C431F5708B7}"/>
     <hyperlink ref="C31" r:id="rId31" tooltip="Hit-Monkey (TV series)" display="https://en.wikipedia.org/wiki/Hit-Monkey_(TV_series)" xr:uid="{DF961AFC-D39C-4EE7-80C2-3E05A4685637}"/>
-    <hyperlink ref="C32" r:id="rId32" tooltip="Moon Girl and Devil Dinosaur" display="https://en.wikipedia.org/wiki/Moon_Girl_and_Devil_Dinosaur" xr:uid="{F0F5034C-3F06-4897-A5E9-551FF35F273F}"/>
+    <hyperlink ref="C33" r:id="rId32" tooltip="Moon Girl and Devil Dinosaur" display="https://en.wikipedia.org/wiki/Moon_Girl_and_Devil_Dinosaur" xr:uid="{F0F5034C-3F06-4897-A5E9-551FF35F273F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId33"/>

</xml_diff>

<commit_message>
facts: update season2 of loki
</commit_message>
<xml_diff>
--- a/facts/step4/all-titles.xlsx
+++ b/facts/step4/all-titles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Dropbox\Coding\marvelsnap-on-screen\facts\step4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DF7A9F-D214-4CB8-8C40-7DA7A9E51B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226A949D-07E6-414E-A00B-997159A52CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
   </bookViews>
   <sheets>
     <sheet name="movie" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="304">
   <si>
     <t>Blade</t>
   </si>
@@ -875,9 +875,6 @@
   </si>
   <si>
     <t>2018–2019</t>
-  </si>
-  <si>
-    <t>2021–2024</t>
   </si>
   <si>
     <t>1992–1997</t>
@@ -1329,7 +1326,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>65</v>
@@ -1341,7 +1338,7 @@
         <v>182</v>
       </c>
       <c r="E1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F1" t="s">
         <v>111</v>
@@ -1352,7 +1349,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B2" s="1">
         <v>1998</v>
@@ -1375,7 +1372,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B3" s="1">
         <v>2000</v>
@@ -1398,7 +1395,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B4" s="1">
         <v>2002</v>
@@ -1421,7 +1418,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B5" s="1">
         <v>2002</v>
@@ -1444,7 +1441,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B6" s="1">
         <v>2003</v>
@@ -1467,7 +1464,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B7" s="1">
         <v>2003</v>
@@ -1490,7 +1487,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B8" s="1">
         <v>2003</v>
@@ -1510,7 +1507,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B9" s="1">
         <v>2004</v>
@@ -1530,7 +1527,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B10" s="1">
         <v>2004</v>
@@ -1553,7 +1550,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B11" s="1">
         <v>2004</v>
@@ -1576,7 +1573,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B12" s="1">
         <v>2005</v>
@@ -1599,7 +1596,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B13" s="1">
         <v>2005</v>
@@ -1622,7 +1619,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B14" s="1">
         <v>2006</v>
@@ -1645,7 +1642,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B15" s="1">
         <v>2007</v>
@@ -1668,7 +1665,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B16" s="1">
         <v>2007</v>
@@ -1691,7 +1688,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B17" s="1">
         <v>2007</v>
@@ -1714,7 +1711,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B18" s="1">
         <v>2008</v>
@@ -1737,7 +1734,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B19" s="1">
         <v>2008</v>
@@ -1760,7 +1757,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B20" s="1">
         <v>2008</v>
@@ -1780,7 +1777,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B21" s="1">
         <v>2008</v>
@@ -1803,7 +1800,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B22" s="1">
         <v>2010</v>
@@ -1826,7 +1823,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B23" s="1">
         <v>2011</v>
@@ -1849,7 +1846,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B24" s="1">
         <v>2011</v>
@@ -1872,7 +1869,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B25" s="1">
         <v>2011</v>
@@ -1895,7 +1892,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B26" s="1">
         <v>2011</v>
@@ -1918,7 +1915,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B27" s="1">
         <v>2012</v>
@@ -1941,7 +1938,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B28" s="1">
         <v>2012</v>
@@ -1964,7 +1961,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B29" s="1">
         <v>2013</v>
@@ -1987,7 +1984,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B30" s="1">
         <v>2013</v>
@@ -2010,7 +2007,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B31" s="1">
         <v>2013</v>
@@ -2033,7 +2030,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B32" s="1">
         <v>2014</v>
@@ -2056,7 +2053,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B33" s="1">
         <v>2014</v>
@@ -2079,7 +2076,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B34" s="1">
         <v>2014</v>
@@ -2102,7 +2099,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B35" s="1">
         <v>2014</v>
@@ -2125,7 +2122,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B36" s="1">
         <v>2015</v>
@@ -2148,7 +2145,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B37" s="1">
         <v>2015</v>
@@ -2171,7 +2168,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B38" s="1">
         <v>2015</v>
@@ -2191,7 +2188,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B39" s="1">
         <v>2016</v>
@@ -2203,7 +2200,7 @@
         <v>219</v>
       </c>
       <c r="E39" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -2214,7 +2211,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B40" s="1">
         <v>2016</v>
@@ -2237,7 +2234,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B41" s="1">
         <v>2016</v>
@@ -2260,7 +2257,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B42" s="1">
         <v>2016</v>
@@ -2283,7 +2280,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B43" s="1">
         <v>2017</v>
@@ -2306,7 +2303,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B44" s="1">
         <v>2017</v>
@@ -2329,7 +2326,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B45" s="1">
         <v>2017</v>
@@ -2352,7 +2349,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>172</v>
@@ -2375,7 +2372,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B47" s="1">
         <v>2018</v>
@@ -2398,7 +2395,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B48" s="1">
         <v>2018</v>
@@ -2421,7 +2418,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B49" s="1">
         <v>2018</v>
@@ -2433,7 +2430,7 @@
         <v>229</v>
       </c>
       <c r="E49" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -2444,7 +2441,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B50" s="1">
         <v>2018</v>
@@ -2467,7 +2464,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B51" s="1">
         <v>2018</v>
@@ -2479,7 +2476,7 @@
         <v>231</v>
       </c>
       <c r="E51" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -2490,7 +2487,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>251</v>
@@ -2502,7 +2499,7 @@
         <v>253</v>
       </c>
       <c r="E52" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -2513,7 +2510,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B53" s="1">
         <v>2019</v>
@@ -2536,7 +2533,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B54" s="1">
         <v>2019</v>
@@ -2559,7 +2556,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B55" s="1">
         <v>2019</v>
@@ -2582,7 +2579,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B56" s="1">
         <v>2019</v>
@@ -2605,7 +2602,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B57" s="1">
         <v>2020</v>
@@ -2628,7 +2625,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B58" s="1">
         <v>2021</v>
@@ -2651,7 +2648,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B59" s="1">
         <v>2021</v>
@@ -2674,7 +2671,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B60" s="1">
         <v>2021</v>
@@ -2686,7 +2683,7 @@
         <v>239</v>
       </c>
       <c r="E60" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F60">
         <v>0</v>
@@ -2697,7 +2694,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B61" s="1">
         <v>2021</v>
@@ -2720,7 +2717,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B62" s="1">
         <v>2021</v>
@@ -2743,7 +2740,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B63" s="1">
         <v>2022</v>
@@ -2766,7 +2763,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B64" s="1">
         <v>2022</v>
@@ -2789,7 +2786,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B65" s="1">
         <v>2022</v>
@@ -2812,7 +2809,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B66" s="1">
         <v>2022</v>
@@ -2835,16 +2832,16 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B67" s="1">
         <v>2022</v>
       </c>
       <c r="C67" t="s">
+        <v>297</v>
+      </c>
+      <c r="D67" t="s">
         <v>298</v>
-      </c>
-      <c r="D67" t="s">
-        <v>299</v>
       </c>
       <c r="E67" t="s">
         <v>113</v>
@@ -2858,16 +2855,16 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B68" s="1">
         <v>2022</v>
       </c>
       <c r="C68" t="s">
+        <v>299</v>
+      </c>
+      <c r="D68" t="s">
         <v>300</v>
-      </c>
-      <c r="D68" t="s">
-        <v>301</v>
       </c>
       <c r="E68" t="s">
         <v>113</v>
@@ -2881,7 +2878,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B69" s="1">
         <v>2023</v>
@@ -2904,7 +2901,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B70" s="1">
         <v>2023</v>
@@ -2927,7 +2924,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>248</v>
@@ -2939,7 +2936,7 @@
         <v>255</v>
       </c>
       <c r="E71" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F71">
         <v>0</v>
@@ -2950,16 +2947,16 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C72" t="s">
+        <v>293</v>
+      </c>
+      <c r="D72" t="s">
         <v>294</v>
-      </c>
-      <c r="D72" t="s">
-        <v>295</v>
       </c>
       <c r="E72" t="s">
         <v>113</v>
@@ -3049,8 +3046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A614F1-7948-4686-8AED-21AFC5640E8C}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3066,7 +3063,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>65</v>
@@ -3078,7 +3075,7 @@
         <v>182</v>
       </c>
       <c r="E1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F1" t="s">
         <v>111</v>
@@ -3089,7 +3086,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B2" s="1">
         <v>2006</v>
@@ -3112,7 +3109,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>274</v>
@@ -3135,7 +3132,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>270</v>
@@ -3158,7 +3155,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>275</v>
@@ -3170,7 +3167,7 @@
         <v>91</v>
       </c>
       <c r="E5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -3181,7 +3178,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>271</v>
@@ -3193,7 +3190,7 @@
         <v>92</v>
       </c>
       <c r="E6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -3204,7 +3201,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>276</v>
@@ -3216,7 +3213,7 @@
         <v>93</v>
       </c>
       <c r="E7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F7">
         <v>2</v>
@@ -3227,7 +3224,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>277</v>
@@ -3247,7 +3244,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>272</v>
@@ -3259,7 +3256,7 @@
         <v>95</v>
       </c>
       <c r="E9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F9">
         <v>2</v>
@@ -3270,7 +3267,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B10" s="1">
         <v>2017</v>
@@ -3282,7 +3279,7 @@
         <v>96</v>
       </c>
       <c r="E10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -3293,7 +3290,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B11" s="1">
         <v>2017</v>
@@ -3316,7 +3313,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>277</v>
@@ -3336,7 +3333,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>277</v>
@@ -3348,7 +3345,7 @@
         <v>99</v>
       </c>
       <c r="E13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -3359,7 +3356,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>277</v>
@@ -3382,7 +3379,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>278</v>
@@ -3405,7 +3402,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B16" s="1">
         <v>2020</v>
@@ -3425,7 +3422,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B17" s="1">
         <v>2021</v>
@@ -3448,7 +3445,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B18" s="1">
         <v>2021</v>
@@ -3471,7 +3468,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B19" s="1">
         <v>2021</v>
@@ -3494,10 +3491,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>279</v>
+        <v>250</v>
       </c>
       <c r="C20" t="s">
         <v>86</v>
@@ -3509,15 +3506,15 @@
         <v>113</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G20">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B21" s="1">
         <v>2022</v>
@@ -3540,7 +3537,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B22" s="1">
         <v>2022</v>
@@ -3563,7 +3560,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B23" s="1">
         <v>2022</v>
@@ -3586,7 +3583,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>248</v>
@@ -3609,16 +3606,16 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C25" t="s">
+        <v>295</v>
+      </c>
+      <c r="D25" t="s">
         <v>296</v>
-      </c>
-      <c r="D25" t="s">
-        <v>297</v>
       </c>
       <c r="E25" t="s">
         <v>113</v>
@@ -3669,7 +3666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3300BA2F-EA0D-4163-B184-5C04F63CD480}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+    <sheetView topLeftCell="C10" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -3686,7 +3683,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>65</v>
@@ -3698,7 +3695,7 @@
         <v>182</v>
       </c>
       <c r="E1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F1" t="s">
         <v>111</v>
@@ -3709,10 +3706,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C2" t="s">
         <v>257</v>
@@ -3729,10 +3726,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C3" t="s">
         <v>258</v>
@@ -3749,10 +3746,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
@@ -3769,10 +3766,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C5" t="s">
         <v>256</v>
@@ -3789,10 +3786,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -3809,7 +3806,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B7" s="1">
         <v>1998</v>
@@ -3829,7 +3826,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>116</v>
@@ -3849,7 +3846,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>118</v>
@@ -3869,7 +3866,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>259</v>
@@ -3889,7 +3886,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B11" s="1">
         <v>2003</v>
@@ -3909,7 +3906,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>260</v>
@@ -3929,7 +3926,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>261</v>
@@ -3949,7 +3946,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B14" s="1">
         <v>2009</v>
@@ -3969,7 +3966,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>262</v>
@@ -3989,7 +3986,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>263</v>
@@ -4009,7 +4006,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>264</v>
@@ -4029,7 +4026,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>265</v>
@@ -4041,7 +4038,7 @@
         <v>157</v>
       </c>
       <c r="E18" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -4052,7 +4049,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>266</v>
@@ -4064,7 +4061,7 @@
         <v>158</v>
       </c>
       <c r="E19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -4075,7 +4072,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>266</v>
@@ -4087,7 +4084,7 @@
         <v>159</v>
       </c>
       <c r="E20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -4098,7 +4095,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>266</v>
@@ -4110,7 +4107,7 @@
         <v>160</v>
       </c>
       <c r="E21" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -4121,7 +4118,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>267</v>
@@ -4141,7 +4138,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>268</v>
@@ -4161,7 +4158,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>269</v>
@@ -4181,7 +4178,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>270</v>
@@ -4193,7 +4190,7 @@
         <v>164</v>
       </c>
       <c r="E25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -4204,7 +4201,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>271</v>
@@ -4224,7 +4221,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>272</v>
@@ -4236,7 +4233,7 @@
         <v>166</v>
       </c>
       <c r="E27" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F27">
         <v>2</v>
@@ -4247,7 +4244,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>273</v>
@@ -4267,7 +4264,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B29" s="1">
         <v>2021</v>
@@ -4287,7 +4284,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>250</v>
@@ -4307,7 +4304,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>249</v>
@@ -4327,16 +4324,16 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B32" t="s">
+        <v>301</v>
+      </c>
+      <c r="C32" t="s">
         <v>302</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>303</v>
-      </c>
-      <c r="D32" t="s">
-        <v>304</v>
       </c>
       <c r="F32">
         <v>2</v>
@@ -4347,7 +4344,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>248</v>

</xml_diff>

<commit_message>
facts: add movie Madam Web
</commit_message>
<xml_diff>
--- a/facts/step4/all-titles.xlsx
+++ b/facts/step4/all-titles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Dropbox\Coding\marvelsnap-on-screen\facts\step4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226A949D-07E6-414E-A00B-997159A52CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C3B1DC-E4A3-4D15-BD44-8A9F0853D38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
   </bookViews>
   <sheets>
     <sheet name="movie" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="307">
   <si>
     <t>Blade</t>
   </si>
@@ -950,6 +950,15 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/I_Am_Groot</t>
+  </si>
+  <si>
+    <t>2024</t>
+  </si>
+  <si>
+    <t>Madame Web</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Madame_Web_(film)</t>
   </si>
 </sst>
 </file>
@@ -1308,23 +1317,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF7CD8B-2C72-4367-8653-A42EAAA710BE}">
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="6.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.5546875" customWidth="1"/>
-    <col min="4" max="4" width="72.5546875" customWidth="1"/>
+    <col min="2" max="2" width="6.5234375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5234375" customWidth="1"/>
+    <col min="4" max="4" width="72.5234375" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1015625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>288</v>
       </c>
@@ -1347,7 +1356,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>289</v>
       </c>
@@ -1370,7 +1379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>289</v>
       </c>
@@ -1393,7 +1402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>289</v>
       </c>
@@ -1416,7 +1425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>289</v>
       </c>
@@ -1439,7 +1448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>289</v>
       </c>
@@ -1462,7 +1471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>289</v>
       </c>
@@ -1485,7 +1494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>289</v>
       </c>
@@ -1505,7 +1514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>289</v>
       </c>
@@ -1525,7 +1534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>289</v>
       </c>
@@ -1548,7 +1557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>289</v>
       </c>
@@ -1571,7 +1580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>289</v>
       </c>
@@ -1594,7 +1603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>289</v>
       </c>
@@ -1617,7 +1626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>289</v>
       </c>
@@ -1640,7 +1649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>289</v>
       </c>
@@ -1663,7 +1672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>289</v>
       </c>
@@ -1686,7 +1695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>289</v>
       </c>
@@ -1709,7 +1718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>289</v>
       </c>
@@ -1732,7 +1741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>289</v>
       </c>
@@ -1755,7 +1764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>289</v>
       </c>
@@ -1775,7 +1784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>289</v>
       </c>
@@ -1798,7 +1807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>289</v>
       </c>
@@ -1821,7 +1830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>289</v>
       </c>
@@ -1844,7 +1853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>289</v>
       </c>
@@ -1867,7 +1876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>289</v>
       </c>
@@ -1890,7 +1899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>289</v>
       </c>
@@ -1913,7 +1922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>289</v>
       </c>
@@ -1936,7 +1945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>289</v>
       </c>
@@ -1959,7 +1968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>289</v>
       </c>
@@ -1982,7 +1991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>289</v>
       </c>
@@ -2005,7 +2014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>289</v>
       </c>
@@ -2028,7 +2037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>289</v>
       </c>
@@ -2051,7 +2060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>289</v>
       </c>
@@ -2074,7 +2083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>289</v>
       </c>
@@ -2097,7 +2106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>289</v>
       </c>
@@ -2120,7 +2129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>289</v>
       </c>
@@ -2143,7 +2152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>289</v>
       </c>
@@ -2166,7 +2175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>289</v>
       </c>
@@ -2186,7 +2195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>289</v>
       </c>
@@ -2209,7 +2218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>289</v>
       </c>
@@ -2232,7 +2241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>289</v>
       </c>
@@ -2255,7 +2264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>289</v>
       </c>
@@ -2278,7 +2287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>289</v>
       </c>
@@ -2301,7 +2310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>289</v>
       </c>
@@ -2324,7 +2333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>289</v>
       </c>
@@ -2347,7 +2356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>289</v>
       </c>
@@ -2370,7 +2379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>289</v>
       </c>
@@ -2393,7 +2402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>289</v>
       </c>
@@ -2416,7 +2425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>289</v>
       </c>
@@ -2439,7 +2448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>289</v>
       </c>
@@ -2462,7 +2471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>289</v>
       </c>
@@ -2485,7 +2494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>289</v>
       </c>
@@ -2508,7 +2517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>289</v>
       </c>
@@ -2531,7 +2540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>289</v>
       </c>
@@ -2554,7 +2563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>289</v>
       </c>
@@ -2577,7 +2586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>289</v>
       </c>
@@ -2600,7 +2609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
         <v>289</v>
       </c>
@@ -2623,7 +2632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>289</v>
       </c>
@@ -2646,7 +2655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
         <v>289</v>
       </c>
@@ -2669,7 +2678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
         <v>289</v>
       </c>
@@ -2692,7 +2701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>289</v>
       </c>
@@ -2715,7 +2724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>289</v>
       </c>
@@ -2738,7 +2747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
         <v>289</v>
       </c>
@@ -2761,7 +2770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>289</v>
       </c>
@@ -2784,7 +2793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
         <v>289</v>
       </c>
@@ -2807,7 +2816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>289</v>
       </c>
@@ -2830,7 +2839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>289</v>
       </c>
@@ -2853,7 +2862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
         <v>289</v>
       </c>
@@ -2876,7 +2885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
         <v>289</v>
       </c>
@@ -2899,7 +2908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
         <v>289</v>
       </c>
@@ -2922,7 +2931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
         <v>289</v>
       </c>
@@ -2945,7 +2954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
         <v>289</v>
       </c>
@@ -2965,6 +2974,29 @@
         <v>0</v>
       </c>
       <c r="G72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" t="s">
+        <v>289</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C73" t="s">
+        <v>305</v>
+      </c>
+      <c r="D73" t="s">
+        <v>306</v>
+      </c>
+      <c r="E73" t="s">
+        <v>180</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
         <v>1</v>
       </c>
     </row>
@@ -3046,22 +3078,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A614F1-7948-4686-8AED-21AFC5640E8C}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.109375" customWidth="1"/>
-    <col min="4" max="4" width="56.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.3125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1015625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.1015625" customWidth="1"/>
+    <col min="4" max="4" width="56.7890625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.41796875" customWidth="1"/>
+    <col min="6" max="6" width="11.1015625" customWidth="1"/>
+    <col min="7" max="7" width="11.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>288</v>
       </c>
@@ -3084,7 +3116,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>291</v>
       </c>
@@ -3107,7 +3139,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>291</v>
       </c>
@@ -3130,7 +3162,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>291</v>
       </c>
@@ -3153,7 +3185,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>291</v>
       </c>
@@ -3176,7 +3208,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>291</v>
       </c>
@@ -3199,7 +3231,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>291</v>
       </c>
@@ -3222,7 +3254,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>291</v>
       </c>
@@ -3242,7 +3274,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>291</v>
       </c>
@@ -3265,7 +3297,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>291</v>
       </c>
@@ -3288,7 +3320,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>291</v>
       </c>
@@ -3311,7 +3343,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>291</v>
       </c>
@@ -3331,7 +3363,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>291</v>
       </c>
@@ -3354,7 +3386,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>291</v>
       </c>
@@ -3377,7 +3409,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>291</v>
       </c>
@@ -3400,7 +3432,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>291</v>
       </c>
@@ -3420,7 +3452,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>291</v>
       </c>
@@ -3443,7 +3475,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>291</v>
       </c>
@@ -3466,7 +3498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>291</v>
       </c>
@@ -3489,7 +3521,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>291</v>
       </c>
@@ -3512,7 +3544,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>291</v>
       </c>
@@ -3535,7 +3567,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>291</v>
       </c>
@@ -3558,7 +3590,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>291</v>
       </c>
@@ -3581,7 +3613,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>291</v>
       </c>
@@ -3604,7 +3636,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>291</v>
       </c>
@@ -3670,18 +3702,18 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.3125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.41796875" style="1" customWidth="1"/>
     <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="68.6640625" customWidth="1"/>
-    <col min="5" max="5" width="6.5546875" customWidth="1"/>
-    <col min="6" max="6" width="12.21875" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="68.68359375" customWidth="1"/>
+    <col min="5" max="5" width="6.5234375" customWidth="1"/>
+    <col min="6" max="6" width="12.20703125" customWidth="1"/>
+    <col min="7" max="7" width="11.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>288</v>
       </c>
@@ -3704,7 +3736,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>290</v>
       </c>
@@ -3724,7 +3756,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>290</v>
       </c>
@@ -3744,7 +3776,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>290</v>
       </c>
@@ -3764,7 +3796,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>290</v>
       </c>
@@ -3784,7 +3816,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>290</v>
       </c>
@@ -3804,7 +3836,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>290</v>
       </c>
@@ -3824,7 +3856,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>290</v>
       </c>
@@ -3844,7 +3876,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>290</v>
       </c>
@@ -3864,7 +3896,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>290</v>
       </c>
@@ -3884,7 +3916,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>290</v>
       </c>
@@ -3904,7 +3936,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>290</v>
       </c>
@@ -3924,7 +3956,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>290</v>
       </c>
@@ -3944,7 +3976,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>290</v>
       </c>
@@ -3964,7 +3996,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>290</v>
       </c>
@@ -3984,7 +4016,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>290</v>
       </c>
@@ -4004,7 +4036,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>290</v>
       </c>
@@ -4024,7 +4056,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>290</v>
       </c>
@@ -4047,7 +4079,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>290</v>
       </c>
@@ -4070,7 +4102,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>290</v>
       </c>
@@ -4093,7 +4125,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>290</v>
       </c>
@@ -4116,7 +4148,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>290</v>
       </c>
@@ -4136,7 +4168,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>290</v>
       </c>
@@ -4156,7 +4188,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>290</v>
       </c>
@@ -4176,7 +4208,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>290</v>
       </c>
@@ -4199,7 +4231,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>290</v>
       </c>
@@ -4219,7 +4251,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>290</v>
       </c>
@@ -4242,7 +4274,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>290</v>
       </c>
@@ -4262,7 +4294,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>290</v>
       </c>
@@ -4282,7 +4314,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>290</v>
       </c>
@@ -4302,7 +4334,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>290</v>
       </c>
@@ -4322,7 +4354,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>290</v>
       </c>
@@ -4342,7 +4374,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>290</v>
       </c>

</xml_diff>

<commit_message>
add movie Deadpool & Wolverine, add card Cassandra Nova
</commit_message>
<xml_diff>
--- a/facts/step4/all-titles.xlsx
+++ b/facts/step4/all-titles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Dropbox\Coding\marvelsnap-on-screen\facts\step4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C3B1DC-E4A3-4D15-BD44-8A9F0853D38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940D4EF9-62B6-453A-BF91-47F1D46B01EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
   </bookViews>
   <sheets>
     <sheet name="movie" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="310">
   <si>
     <t>Blade</t>
   </si>
@@ -959,6 +959,15 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/Madame_Web_(film)</t>
+  </si>
+  <si>
+    <t>Deadpool &amp; Wolverine</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Deadpool_%26_Wolverine</t>
+  </si>
+  <si>
+    <t>fox-x-men,deadpool, mcu</t>
   </si>
 </sst>
 </file>
@@ -1317,10 +1326,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF7CD8B-2C72-4367-8653-A42EAAA710BE}">
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2997,6 +3006,29 @@
         <v>0</v>
       </c>
       <c r="G73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" t="s">
+        <v>289</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C74" t="s">
+        <v>307</v>
+      </c>
+      <c r="D74" t="s">
+        <v>308</v>
+      </c>
+      <c r="E74" t="s">
+        <v>309</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add new animated show x-men '97
</commit_message>
<xml_diff>
--- a/facts/step4/all-titles.xlsx
+++ b/facts/step4/all-titles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Dropbox\Coding\marvelsnap-on-screen\facts\step4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940D4EF9-62B6-453A-BF91-47F1D46B01EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880265CB-3F85-4C92-80ED-7BD82891BFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
   </bookViews>
   <sheets>
     <sheet name="movie" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="312">
   <si>
     <t>Blade</t>
   </si>
@@ -968,6 +968,12 @@
   </si>
   <si>
     <t>fox-x-men,deadpool, mcu</t>
+  </si>
+  <si>
+    <t>X-Men '97</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/X-Men_%2797</t>
   </si>
 </sst>
 </file>
@@ -1328,8 +1334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF7CD8B-2C72-4367-8653-A42EAAA710BE}">
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="G74" sqref="G74"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3728,10 +3734,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3300BA2F-EA0D-4163-B184-5C04F63CD480}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4424,6 +4430,26 @@
       </c>
       <c r="G33">
         <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>290</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C34" t="s">
+        <v>310</v>
+      </c>
+      <c r="D34" t="s">
+        <v>311</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add movie "'2024 Venom: the last dance', add card Toxin
</commit_message>
<xml_diff>
--- a/facts/step4/all-titles.xlsx
+++ b/facts/step4/all-titles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Dropbox\Coding\marvelsnap-on-screen\facts\step4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880265CB-3F85-4C92-80ED-7BD82891BFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5A7774-F056-4604-9966-E9FC0A23EB8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
   </bookViews>
   <sheets>
     <sheet name="movie" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="314">
   <si>
     <t>Blade</t>
   </si>
@@ -974,6 +974,12 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/X-Men_%2797</t>
+  </si>
+  <si>
+    <t>Venom: The Last Dance</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Venom:_The_Last_Dance</t>
   </si>
 </sst>
 </file>
@@ -1332,10 +1338,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF7CD8B-2C72-4367-8653-A42EAAA710BE}">
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="H75" sqref="H75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3035,6 +3041,29 @@
         <v>0</v>
       </c>
       <c r="G74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" t="s">
+        <v>289</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C75" t="s">
+        <v>312</v>
+      </c>
+      <c r="D75" t="s">
+        <v>313</v>
+      </c>
+      <c r="E75" t="s">
+        <v>284</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
         <v>1</v>
       </c>
     </row>
@@ -3736,8 +3765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3300BA2F-EA0D-4163-B184-5C04F63CD480}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
facts: add movie Captain America: Brave New World
</commit_message>
<xml_diff>
--- a/facts/step4/all-titles.xlsx
+++ b/facts/step4/all-titles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Dropbox\Coding\marvelsnap-on-screen\facts\step4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9B2B28-A99B-412B-A523-DF2848E4F9FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909B0D21-28D3-4C2B-9F10-1B3BD3E7FA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="1" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
   </bookViews>
   <sheets>
     <sheet name="movie" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="321">
   <si>
     <t>Blade</t>
   </si>
@@ -992,6 +992,15 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/Agatha_All_Along_(miniseries)</t>
+  </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t>Captain America: Brave New World</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Captain_America:_Brave_New_World</t>
   </si>
 </sst>
 </file>
@@ -1350,10 +1359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF7CD8B-2C72-4367-8653-A42EAAA710BE}">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="G76" sqref="G76"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3099,6 +3108,29 @@
         <v>0</v>
       </c>
       <c r="G76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" t="s">
+        <v>289</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C77" t="s">
+        <v>319</v>
+      </c>
+      <c r="D77" t="s">
+        <v>320</v>
+      </c>
+      <c r="E77" t="s">
+        <v>113</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
         <v>1</v>
       </c>
     </row>
@@ -3180,7 +3212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A614F1-7948-4686-8AED-21AFC5640E8C}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add new show Daredevil: Born Again
</commit_message>
<xml_diff>
--- a/facts/step4/all-titles.xlsx
+++ b/facts/step4/all-titles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Dropbox\Coding\marvelsnap-on-screen\facts\step4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB33713F-2B29-4FE2-BC2D-E525321295EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD3B5FC-F175-438E-98DD-97C6B98DA1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="1" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
   </bookViews>
   <sheets>
     <sheet name="movie" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="325">
   <si>
     <t>Blade</t>
   </si>
@@ -1007,6 +1007,12 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/Thunderbolts*</t>
+  </si>
+  <si>
+    <t>Daredevil: Born Again</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Daredevil:_Born_Again</t>
   </si>
 </sst>
 </file>
@@ -1367,7 +1373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF7CD8B-2C72-4367-8653-A42EAAA710BE}">
   <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+    <sheetView topLeftCell="A53" workbookViewId="0">
       <selection activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
@@ -3239,10 +3245,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A614F1-7948-4686-8AED-21AFC5640E8C}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3842,6 +3848,29 @@
         <v>1</v>
       </c>
       <c r="G26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>291</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C27" t="s">
+        <v>323</v>
+      </c>
+      <c r="D27" t="s">
+        <v>324</v>
+      </c>
+      <c r="E27" t="s">
+        <v>113</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add movie "The Fantastic Four: First Steps"
</commit_message>
<xml_diff>
--- a/facts/step4/all-titles.xlsx
+++ b/facts/step4/all-titles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Dropbox\Coding\marvelsnap-on-screen\facts\step4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD3B5FC-F175-438E-98DD-97C6B98DA1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB844A6E-8861-449B-873A-06DACA63C621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="1" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
   </bookViews>
   <sheets>
     <sheet name="movie" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="327">
   <si>
     <t>Blade</t>
   </si>
@@ -1013,6 +1013,12 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/Daredevil:_Born_Again</t>
+  </si>
+  <si>
+    <t>The Fantastic Four: First Steps</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/The_Fantastic_Four:_First_Steps</t>
   </si>
 </sst>
 </file>
@@ -1371,10 +1377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF7CD8B-2C72-4367-8653-A42EAAA710BE}">
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="G78" sqref="G78"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3166,6 +3172,29 @@
         <v>0</v>
       </c>
       <c r="G78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" t="s">
+        <v>289</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C79" t="s">
+        <v>325</v>
+      </c>
+      <c r="D79" t="s">
+        <v>326</v>
+      </c>
+      <c r="E79" t="s">
+        <v>113</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
         <v>1</v>
       </c>
     </row>
@@ -3247,7 +3276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A614F1-7948-4686-8AED-21AFC5640E8C}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update season and episode count for hit-monkey
</commit_message>
<xml_diff>
--- a/facts/step4/all-titles.xlsx
+++ b/facts/step4/all-titles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Dropbox\Coding\marvelsnap-on-screen\facts\step4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB844A6E-8861-449B-873A-06DACA63C621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F560ED9-8212-4999-B624-DE3609B11A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
   </bookViews>
   <sheets>
     <sheet name="movie" sheetId="1" r:id="rId1"/>
@@ -1379,7 +1379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF7CD8B-2C72-4367-8653-A42EAAA710BE}">
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -3942,8 +3942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3300BA2F-EA0D-4163-B184-5C04F63CD480}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4592,10 +4592,10 @@
         <v>170</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G31">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Add show "Your Friendly Neighborhood Spider-Man" and "Iron Man and His Awesome Friends"
</commit_message>
<xml_diff>
--- a/facts/step4/all-titles.xlsx
+++ b/facts/step4/all-titles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Dropbox\Coding\marvelsnap-on-screen\facts\step4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F560ED9-8212-4999-B624-DE3609B11A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85A8CC2-AC4D-41D4-89C6-C93212B0C67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="331">
   <si>
     <t>Blade</t>
   </si>
@@ -1019,6 +1019,18 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/The_Fantastic_Four:_First_Steps</t>
+  </si>
+  <si>
+    <t>Your Friendly Neighborhood Spider-Man</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Your_Friendly_Neighborhood_Spider-Man</t>
+  </si>
+  <si>
+    <t>Iron Man and His Awesome Friends</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Iron_Man_and_His_Awesome_Friends</t>
   </si>
 </sst>
 </file>
@@ -3940,10 +3952,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3300BA2F-EA0D-4163-B184-5C04F63CD480}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4655,6 +4667,46 @@
         <v>1</v>
       </c>
       <c r="G34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>290</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C35" t="s">
+        <v>327</v>
+      </c>
+      <c r="D35" t="s">
+        <v>328</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>290</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C36" t="s">
+        <v>329</v>
+      </c>
+      <c r="D36" t="s">
+        <v>330</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add 2025 show "Ironheart" and "Eyes of Wakanda"
</commit_message>
<xml_diff>
--- a/facts/step4/all-titles.xlsx
+++ b/facts/step4/all-titles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Dropbox\Coding\marvelsnap-on-screen\facts\step4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85A8CC2-AC4D-41D4-89C6-C93212B0C67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10AC785-14F3-495D-A13F-B43FA4FD3BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
   </bookViews>
   <sheets>
     <sheet name="movie" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="335">
   <si>
     <t>Blade</t>
   </si>
@@ -1031,6 +1031,18 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/Iron_Man_and_His_Awesome_Friends</t>
+  </si>
+  <si>
+    <t>Eyes of Wakanda</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Eyes_of_Wakanda</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Ironheart_(miniseries)</t>
+  </si>
+  <si>
+    <t>Ironheart</t>
   </si>
 </sst>
 </file>
@@ -3286,10 +3298,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A614F1-7948-4686-8AED-21AFC5640E8C}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3913,6 +3925,29 @@
       </c>
       <c r="G27">
         <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>291</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C28" t="s">
+        <v>334</v>
+      </c>
+      <c r="D28" t="s">
+        <v>333</v>
+      </c>
+      <c r="E28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -3952,10 +3987,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3300BA2F-EA0D-4163-B184-5C04F63CD480}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4708,6 +4743,26 @@
       </c>
       <c r="G36">
         <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>290</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C37" t="s">
+        <v>331</v>
+      </c>
+      <c r="D37" t="s">
+        <v>332</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improve spidey and his friends
</commit_message>
<xml_diff>
--- a/facts/step4/all-titles.xlsx
+++ b/facts/step4/all-titles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Dropbox\Coding\marvelsnap-on-screen\facts\step4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10AC785-14F3-495D-A13F-B43FA4FD3BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE815A6D-24AE-4640-97FC-7AE617D42096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
   </bookViews>
   <sheets>
     <sheet name="movie" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="336">
   <si>
     <t>Blade</t>
   </si>
@@ -1043,6 +1043,9 @@
   </si>
   <si>
     <t>Ironheart</t>
+  </si>
+  <si>
+    <t>2021–2025</t>
   </si>
 </sst>
 </file>
@@ -3300,7 +3303,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A614F1-7948-4686-8AED-21AFC5640E8C}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -3989,8 +3992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3300BA2F-EA0D-4163-B184-5C04F63CD480}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4610,7 +4613,7 @@
         <v>290</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>250</v>
+        <v>335</v>
       </c>
       <c r="C30" t="s">
         <v>138</v>
@@ -4619,10 +4622,10 @@
         <v>169</v>
       </c>
       <c r="F30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G30">
-        <v>47</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Add show "Marvel Zombies"
</commit_message>
<xml_diff>
--- a/facts/step4/all-titles.xlsx
+++ b/facts/step4/all-titles.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Dropbox\Coding\marvelsnap-on-screen\facts\step4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE815A6D-24AE-4640-97FC-7AE617D42096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6197ED4-F63E-488B-8B8D-4F7F677B8788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="338">
   <si>
     <t>Blade</t>
   </si>
@@ -1046,6 +1046,12 @@
   </si>
   <si>
     <t>2021–2025</t>
+  </si>
+  <si>
+    <t>Marvel Zombies</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Marvel_Zombies_(miniseries)</t>
   </si>
 </sst>
 </file>
@@ -3303,7 +3309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A614F1-7948-4686-8AED-21AFC5640E8C}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -3990,10 +3996,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3300BA2F-EA0D-4163-B184-5C04F63CD480}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4765,6 +4771,26 @@
         <v>1</v>
       </c>
       <c r="G37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>290</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C38" t="s">
+        <v>336</v>
+      </c>
+      <c r="D38" t="s">
+        <v>337</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
         <v>4</v>
       </c>
     </row>

</xml_diff>